<commit_message>
Working on autocreating the short stat block for NPCs
</commit_message>
<xml_diff>
--- a/SupersNew/characters/Banshee.xlsx
+++ b/SupersNew/characters/Banshee.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jom128/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rb\SupersNew\characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1DD89B8-5835-F54A-AFCC-AF93986FC828}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="3620" windowWidth="20660" windowHeight="10420" xr2:uid="{C5BDF303-2A10-428A-B5FA-9C2DEF49E8B6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="Character Sheet" sheetId="1" r:id="rId1"/>
@@ -400,7 +399,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,7 +430,7 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="1"/>
@@ -603,6 +602,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -610,7 +610,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -665,89 +664,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63B25935-A080-0847-9579-9BA47B8CBEAF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8915400" y="190500"/>
-          <a:ext cx="1955800" cy="1104900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>To Use, fill in your stats in the highlighted colum, then select your fighting profile from the drop down.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Powers are manual for the time being.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1046,72 +962,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AFC3A5-DB28-4F5E-8A77-AD87DC2FBB2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:I33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
-    <col min="8" max="8" width="34.33203125" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="10" t="s">
         <v>49</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1122,7 +1038,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1136,7 +1052,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -1160,7 +1076,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1184,7 +1100,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1204,11 +1120,11 @@
         <v>10.5</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -1232,7 +1148,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1254,7 +1170,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -1276,7 +1192,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1293,7 +1209,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1310,7 +1226,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1320,7 +1236,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>73</v>
       </c>
@@ -1332,14 +1248,14 @@
       <c r="D15" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="9" t="s">
         <v>78</v>
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>74</v>
       </c>
@@ -1350,10 +1266,10 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>72</v>
       </c>
@@ -1365,20 +1281,20 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="11"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="11"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>1</v>
       </c>
@@ -1390,7 +1306,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
@@ -1419,7 +1335,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>49</v>
       </c>
@@ -1448,7 +1364,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -1461,7 +1377,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -1474,7 +1390,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>95</v>
       </c>
@@ -1503,7 +1419,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -1516,7 +1432,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -1529,7 +1445,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>99</v>
       </c>
@@ -1558,7 +1474,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>104</v>
       </c>
@@ -1587,7 +1503,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>107</v>
       </c>
@@ -1616,7 +1532,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -1629,7 +1545,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -1642,7 +1558,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="53" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>114</v>
       </c>
@@ -1671,7 +1587,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>117</v>
       </c>
@@ -1702,14 +1618,11 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="H21:H23"/>
@@ -1726,19 +1639,21 @@
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="E21:E23"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F6F6D3B2-7E06-412F-84AC-15F1D0EF35D1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Fighting Profiles'!$A$2:$A$34</xm:f>
           </x14:formula1>
@@ -1751,23 +1666,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4CCAA4-8C1E-4D1B-BBAE-A9818AB55217}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1790,7 +1705,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1818,7 +1733,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1846,7 +1761,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1874,7 +1789,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1899,7 +1814,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1924,7 +1839,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1952,7 +1867,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1980,7 +1895,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -2008,7 +1923,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -2036,7 +1951,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -2064,7 +1979,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2092,7 +2007,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -2120,7 +2035,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2145,7 +2060,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2170,7 +2085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2195,7 +2110,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2220,7 +2135,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2245,7 +2160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2270,7 +2185,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2295,7 +2210,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2320,7 +2235,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2345,7 +2260,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -2370,7 +2285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2395,7 +2310,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -2420,7 +2335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2445,7 +2360,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -2470,7 +2385,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2495,7 +2410,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2520,7 +2435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2545,7 +2460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -2570,7 +2485,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2595,7 +2510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -2620,7 +2535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -2646,7 +2561,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F34">
+  <sortState ref="A2:F34">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>